<commit_message>
Investment 7 Years Plan
Charges site

https://select.finology.in/broker/groww/calculator
</commit_message>
<xml_diff>
--- a/Invertment Data.xlsx
+++ b/Invertment Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t>Month</t>
   </si>
@@ -86,15 +86,45 @@
   <si>
     <t>Return Per Day/Trading for 15 days</t>
   </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Charges Site</t>
+  </si>
+  <si>
+    <t>https://select.finology.in/broker/groww/calculator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,10 +197,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -178,8 +210,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +721,7 @@
     <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.54296875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,6 +732,12 @@
       <c r="B1">
         <v>10000</v>
       </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -717,7 +761,7 @@
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -749,10 +793,10 @@
         <v>688.2</v>
       </c>
       <c r="G3" s="4">
-        <f>((B3/100)*C3)-F3</f>
+        <f t="shared" ref="G3:G14" si="0">((B3/100)*C3)-F3</f>
         <v>811.8</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="9">
         <f>B3+G3</f>
         <v>10811.8</v>
       </c>
@@ -783,23 +827,23 @@
         <v>22.19</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" ref="F4:F14" si="0">C4*(D4+E4)</f>
+        <f t="shared" ref="F4:F14" si="1">C4*(D4+E4)</f>
         <v>688.2</v>
       </c>
       <c r="G4" s="4">
-        <f>((B4/100)*C4)-F4</f>
+        <f t="shared" si="0"/>
         <v>933.56999999999994</v>
       </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H8" si="1">B4+G4</f>
+      <c r="H4" s="9">
+        <f t="shared" ref="H4:H8" si="2">B4+G4</f>
         <v>11745.369999999999</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I14" si="2">C4/4</f>
+        <f t="shared" ref="I4:I14" si="3">C4/4</f>
         <v>3.75</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J14" si="3">C4/15</f>
+        <f t="shared" ref="J4:J14" si="4">C4/15</f>
         <v>1</v>
       </c>
     </row>
@@ -808,7 +852,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:B8" si="4">H4</f>
+        <f t="shared" ref="B5:B8" si="5">H4</f>
         <v>11745.369999999999</v>
       </c>
       <c r="C5" s="4">
@@ -821,23 +865,23 @@
         <v>22.19</v>
       </c>
       <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G5" s="4">
-        <f>((B5/100)*C5)-F5</f>
         <v>1073.6054999999997</v>
       </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
+      <c r="H5" s="9">
+        <f t="shared" si="2"/>
         <v>12818.975499999999</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -846,36 +890,36 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
+        <f t="shared" si="5"/>
+        <v>12818.975499999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E6" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>1234.6463249999999</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="2"/>
+        <v>14053.621824999998</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>12818.975499999999</v>
-      </c>
-      <c r="C6" s="4">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E6" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G6" s="4">
-        <f>((B6/100)*C6)-F6</f>
-        <v>1234.6463249999999</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>14053.621824999998</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="2"/>
-        <v>3.75</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -884,36 +928,36 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
+        <f t="shared" si="5"/>
+        <v>14053.621824999998</v>
+      </c>
+      <c r="C7" s="4">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E7" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>1419.84327375</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="2"/>
+        <v>15473.465098749999</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>14053.621824999998</v>
-      </c>
-      <c r="C7" s="4">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E7" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G7" s="4">
-        <f>((B7/100)*C7)-F7</f>
-        <v>1419.84327375</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>15473.465098749999</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="2"/>
-        <v>3.75</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -922,36 +966,36 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
+        <f t="shared" si="5"/>
+        <v>15473.465098749999</v>
+      </c>
+      <c r="C8" s="4">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E8" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>1632.8197648124999</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="2"/>
+        <v>17106.284863562498</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>15473.465098749999</v>
-      </c>
-      <c r="C8" s="4">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E8" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G8" s="4">
-        <f>((B8/100)*C8)-F8</f>
-        <v>1632.8197648124999</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="1"/>
-        <v>17106.284863562498</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>3.75</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -960,7 +1004,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" ref="B9:B14" si="5">H8</f>
+        <f t="shared" ref="B9:B14" si="6">H8</f>
         <v>17106.284863562498</v>
       </c>
       <c r="C9" s="4">
@@ -973,23 +1017,23 @@
         <v>22.19</v>
       </c>
       <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G9" s="4">
-        <f>((B9/100)*C9)-F9</f>
         <v>1877.7427295343748</v>
       </c>
-      <c r="H9" s="4">
-        <f t="shared" ref="H9:H14" si="6">B9+G9</f>
+      <c r="H9" s="9">
+        <f t="shared" ref="H9:H14" si="7">B9+G9</f>
         <v>18984.027593096871</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -998,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18984.027593096871</v>
       </c>
       <c r="C10" s="4">
@@ -1011,23 +1055,23 @@
         <v>22.19</v>
       </c>
       <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G10" s="4">
-        <f>((B10/100)*C10)-F10</f>
         <v>2159.4041389645308</v>
       </c>
-      <c r="H10" s="4">
-        <f t="shared" si="6"/>
+      <c r="H10" s="9">
+        <f t="shared" si="7"/>
         <v>21143.431732061403</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1036,7 +1080,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21143.431732061403</v>
       </c>
       <c r="C11" s="4">
@@ -1049,23 +1093,23 @@
         <v>22.19</v>
       </c>
       <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G11" s="4">
-        <f>((B11/100)*C11)-F11</f>
         <v>2483.31475980921</v>
       </c>
-      <c r="H11" s="4">
-        <f t="shared" si="6"/>
+      <c r="H11" s="9">
+        <f t="shared" si="7"/>
         <v>23626.746491870614</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1074,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23626.746491870614</v>
       </c>
       <c r="C12" s="4">
@@ -1087,23 +1131,23 @@
         <v>22.19</v>
       </c>
       <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G12" s="4">
-        <f>((B12/100)*C12)-F12</f>
         <v>2855.8119737805919</v>
       </c>
-      <c r="H12" s="4">
-        <f t="shared" si="6"/>
+      <c r="H12" s="9">
+        <f t="shared" si="7"/>
         <v>26482.558465651207</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1112,7 +1156,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26482.558465651207</v>
       </c>
       <c r="C13" s="4">
@@ -1125,23 +1169,23 @@
         <v>22.19</v>
       </c>
       <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G13" s="4">
-        <f>((B13/100)*C13)-F13</f>
         <v>3284.1837698476811</v>
       </c>
-      <c r="H13" s="4">
-        <f t="shared" si="6"/>
+      <c r="H13" s="9">
+        <f t="shared" si="7"/>
         <v>29766.742235498888</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1150,7 +1194,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29766.742235498888</v>
       </c>
       <c r="C14" s="4">
@@ -1163,23 +1207,23 @@
         <v>22.19</v>
       </c>
       <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>688.2</v>
+      </c>
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>688.2</v>
-      </c>
-      <c r="G14" s="4">
-        <f>((B14/100)*C14)-F14</f>
         <v>3776.8113353248336</v>
       </c>
-      <c r="H14" s="4">
-        <f t="shared" si="6"/>
+      <c r="H14" s="9">
+        <f t="shared" si="7"/>
         <v>33543.553570823722</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1219,7 +1263,7 @@
       <c r="G19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -1251,10 +1295,10 @@
         <v>688.2</v>
       </c>
       <c r="G20" s="4">
-        <f>((B20/100)*C20)-F20</f>
+        <f t="shared" ref="G20:G31" si="8">((B20/100)*C20)-F20</f>
         <v>4343.3330356235592</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="9">
         <f>B20+G20</f>
         <v>37886.886606447282</v>
       </c>
@@ -1285,23 +1329,23 @@
         <v>22.19</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" ref="F21:F31" si="7">C21*(D21+E21)</f>
+        <f t="shared" ref="F21:F31" si="9">C21*(D21+E21)</f>
         <v>688.2</v>
       </c>
       <c r="G21" s="4">
-        <f>((B21/100)*C21)-F21</f>
+        <f t="shared" si="8"/>
         <v>4994.832990967092</v>
       </c>
-      <c r="H21" s="4">
-        <f t="shared" ref="H21:H31" si="8">B21+G21</f>
+      <c r="H21" s="9">
+        <f t="shared" ref="H21:H31" si="10">B21+G21</f>
         <v>42881.719597414376</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" ref="I21:I31" si="9">C21/4</f>
+        <f t="shared" ref="I21:I31" si="11">C21/4</f>
         <v>3.75</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" ref="J21:J31" si="10">C21/15</f>
+        <f t="shared" ref="J21:J31" si="12">C21/15</f>
         <v>1</v>
       </c>
     </row>
@@ -1310,7 +1354,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="4">
-        <f t="shared" ref="B22:B31" si="11">H21</f>
+        <f t="shared" ref="B22:B31" si="13">H21</f>
         <v>42881.719597414376</v>
       </c>
       <c r="C22" s="4">
@@ -1323,23 +1367,23 @@
         <v>22.19</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>688.2</v>
       </c>
       <c r="G22" s="4">
-        <f>((B22/100)*C22)-F22</f>
+        <f t="shared" si="8"/>
         <v>5744.0579396121566</v>
       </c>
-      <c r="H22" s="4">
-        <f t="shared" si="8"/>
+      <c r="H22" s="9">
+        <f t="shared" si="10"/>
         <v>48625.77753702653</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.75</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1348,36 +1392,36 @@
         <v>4</v>
       </c>
       <c r="B23" s="4">
+        <f t="shared" si="13"/>
+        <v>48625.77753702653</v>
+      </c>
+      <c r="C23" s="4">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E23" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="8"/>
+        <v>6605.6666305539793</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="10"/>
+        <v>55231.444167580506</v>
+      </c>
+      <c r="I23" s="4">
         <f t="shared" si="11"/>
-        <v>48625.77753702653</v>
-      </c>
-      <c r="C23" s="4">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E23" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F23" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G23" s="4">
-        <f>((B23/100)*C23)-F23</f>
-        <v>6605.6666305539793</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="8"/>
-        <v>55231.444167580506</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1386,36 +1430,36 @@
         <v>5</v>
       </c>
       <c r="B24" s="4">
+        <f t="shared" si="13"/>
+        <v>55231.444167580506</v>
+      </c>
+      <c r="C24" s="4">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E24" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="8"/>
+        <v>7596.5166251370765</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="10"/>
+        <v>62827.960792717582</v>
+      </c>
+      <c r="I24" s="4">
         <f t="shared" si="11"/>
-        <v>55231.444167580506</v>
-      </c>
-      <c r="C24" s="4">
-        <v>15</v>
-      </c>
-      <c r="D24" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E24" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G24" s="4">
-        <f>((B24/100)*C24)-F24</f>
-        <v>7596.5166251370765</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="8"/>
-        <v>62827.960792717582</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1424,36 +1468,36 @@
         <v>6</v>
       </c>
       <c r="B25" s="4">
+        <f t="shared" si="13"/>
+        <v>62827.960792717582</v>
+      </c>
+      <c r="C25" s="4">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E25" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="8"/>
+        <v>8735.9941189076362</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="10"/>
+        <v>71563.954911625216</v>
+      </c>
+      <c r="I25" s="4">
         <f t="shared" si="11"/>
-        <v>62827.960792717582</v>
-      </c>
-      <c r="C25" s="4">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E25" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G25" s="4">
-        <f>((B25/100)*C25)-F25</f>
-        <v>8735.9941189076362</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="8"/>
-        <v>71563.954911625216</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1462,36 +1506,36 @@
         <v>7</v>
       </c>
       <c r="B26" s="4">
+        <f t="shared" si="13"/>
+        <v>71563.954911625216</v>
+      </c>
+      <c r="C26" s="4">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E26" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="8"/>
+        <v>10046.393236743781</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="10"/>
+        <v>81610.348148368997</v>
+      </c>
+      <c r="I26" s="4">
         <f t="shared" si="11"/>
-        <v>71563.954911625216</v>
-      </c>
-      <c r="C26" s="4">
-        <v>15</v>
-      </c>
-      <c r="D26" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E26" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F26" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G26" s="4">
-        <f>((B26/100)*C26)-F26</f>
-        <v>10046.393236743781</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="8"/>
-        <v>81610.348148368997</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1500,36 +1544,36 @@
         <v>8</v>
       </c>
       <c r="B27" s="4">
+        <f t="shared" si="13"/>
+        <v>81610.348148368997</v>
+      </c>
+      <c r="C27" s="4">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E27" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="8"/>
+        <v>11553.352222255349</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="10"/>
+        <v>93163.700370624341</v>
+      </c>
+      <c r="I27" s="4">
         <f t="shared" si="11"/>
-        <v>81610.348148368997</v>
-      </c>
-      <c r="C27" s="4">
-        <v>15</v>
-      </c>
-      <c r="D27" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E27" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F27" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G27" s="4">
-        <f>((B27/100)*C27)-F27</f>
-        <v>11553.352222255349</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="8"/>
-        <v>93163.700370624341</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1538,36 +1582,36 @@
         <v>9</v>
       </c>
       <c r="B28" s="4">
+        <f t="shared" si="13"/>
+        <v>93163.700370624341</v>
+      </c>
+      <c r="C28" s="4">
+        <v>15</v>
+      </c>
+      <c r="D28" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E28" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="8"/>
+        <v>13286.355055593649</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="10"/>
+        <v>106450.05542621799</v>
+      </c>
+      <c r="I28" s="4">
         <f t="shared" si="11"/>
-        <v>93163.700370624341</v>
-      </c>
-      <c r="C28" s="4">
-        <v>15</v>
-      </c>
-      <c r="D28" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E28" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F28" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G28" s="4">
-        <f>((B28/100)*C28)-F28</f>
-        <v>13286.355055593649</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="8"/>
-        <v>106450.05542621799</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J28" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1576,36 +1620,36 @@
         <v>10</v>
       </c>
       <c r="B29" s="4">
+        <f t="shared" si="13"/>
+        <v>106450.05542621799</v>
+      </c>
+      <c r="C29" s="4">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E29" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="8"/>
+        <v>15279.308313932699</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="10"/>
+        <v>121729.3637401507</v>
+      </c>
+      <c r="I29" s="4">
         <f t="shared" si="11"/>
-        <v>106450.05542621799</v>
-      </c>
-      <c r="C29" s="4">
-        <v>15</v>
-      </c>
-      <c r="D29" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E29" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F29" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G29" s="4">
-        <f>((B29/100)*C29)-F29</f>
-        <v>15279.308313932699</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="8"/>
-        <v>121729.3637401507</v>
-      </c>
-      <c r="I29" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1614,36 +1658,36 @@
         <v>11</v>
       </c>
       <c r="B30" s="4">
+        <f t="shared" si="13"/>
+        <v>121729.3637401507</v>
+      </c>
+      <c r="C30" s="4">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E30" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="8"/>
+        <v>17571.204561022605</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="10"/>
+        <v>139300.56830117331</v>
+      </c>
+      <c r="I30" s="4">
         <f t="shared" si="11"/>
-        <v>121729.3637401507</v>
-      </c>
-      <c r="C30" s="4">
-        <v>15</v>
-      </c>
-      <c r="D30" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E30" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G30" s="4">
-        <f>((B30/100)*C30)-F30</f>
-        <v>17571.204561022605</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="8"/>
-        <v>139300.56830117331</v>
-      </c>
-      <c r="I30" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1652,36 +1696,36 @@
         <v>12</v>
       </c>
       <c r="B31" s="4">
+        <f t="shared" si="13"/>
+        <v>139300.56830117331</v>
+      </c>
+      <c r="C31" s="4">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E31" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="9"/>
+        <v>688.2</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="8"/>
+        <v>20206.885245175996</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="10"/>
+        <v>159507.45354634931</v>
+      </c>
+      <c r="I31" s="4">
         <f t="shared" si="11"/>
-        <v>139300.56830117331</v>
-      </c>
-      <c r="C31" s="4">
-        <v>15</v>
-      </c>
-      <c r="D31" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E31" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F31" s="4">
-        <f t="shared" si="7"/>
-        <v>688.2</v>
-      </c>
-      <c r="G31" s="4">
-        <f>((B31/100)*C31)-F31</f>
-        <v>20206.885245175996</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="8"/>
-        <v>159507.45354634931</v>
-      </c>
-      <c r="I31" s="4">
-        <f t="shared" si="9"/>
         <v>3.75</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -1721,7 +1765,7 @@
       <c r="G36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I36" s="6" t="s">
@@ -1753,10 +1797,10 @@
         <v>688.2</v>
       </c>
       <c r="G37" s="4">
-        <f>((B37/100)*C37)-F37</f>
+        <f t="shared" ref="G37:G48" si="14">((B37/100)*C37)-F37</f>
         <v>23237.918031952395</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="9">
         <f>B37+G37</f>
         <v>182745.37157830171</v>
       </c>
@@ -1787,23 +1831,23 @@
         <v>22.19</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" ref="F38:F48" si="12">C38*(D38+E38)</f>
+        <f t="shared" ref="F38:F48" si="15">C38*(D38+E38)</f>
         <v>688.2</v>
       </c>
       <c r="G38" s="4">
-        <f>((B38/100)*C38)-F38</f>
+        <f t="shared" si="14"/>
         <v>26723.605736745256</v>
       </c>
-      <c r="H38" s="4">
-        <f t="shared" ref="H38:H48" si="13">B38+G38</f>
+      <c r="H38" s="9">
+        <f t="shared" ref="H38:H48" si="16">B38+G38</f>
         <v>209468.97731504697</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I38:I48" si="14">C38/4</f>
+        <f t="shared" ref="I38:I48" si="17">C38/4</f>
         <v>3.75</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:J48" si="15">C38/15</f>
+        <f t="shared" ref="J38:J48" si="18">C38/15</f>
         <v>1</v>
       </c>
     </row>
@@ -1812,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="4">
-        <f t="shared" ref="B39:B48" si="16">H38</f>
+        <f t="shared" ref="B39:B48" si="19">H38</f>
         <v>209468.97731504697</v>
       </c>
       <c r="C39" s="4">
@@ -1825,23 +1869,23 @@
         <v>22.19</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>688.2</v>
       </c>
       <c r="G39" s="4">
-        <f>((B39/100)*C39)-F39</f>
+        <f t="shared" si="14"/>
         <v>30732.146597257044</v>
       </c>
-      <c r="H39" s="4">
-        <f t="shared" si="13"/>
+      <c r="H39" s="9">
+        <f t="shared" si="16"/>
         <v>240201.123912304</v>
       </c>
       <c r="I39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -1850,36 +1894,36 @@
         <v>4</v>
       </c>
       <c r="B40" s="4">
+        <f t="shared" si="19"/>
+        <v>240201.123912304</v>
+      </c>
+      <c r="C40" s="4">
+        <v>15</v>
+      </c>
+      <c r="D40" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E40" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F40" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="14"/>
+        <v>35341.9685868456</v>
+      </c>
+      <c r="H40" s="9">
         <f t="shared" si="16"/>
-        <v>240201.123912304</v>
-      </c>
-      <c r="C40" s="4">
-        <v>15</v>
-      </c>
-      <c r="D40" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E40" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F40" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G40" s="4">
-        <f>((B40/100)*C40)-F40</f>
-        <v>35341.9685868456</v>
-      </c>
-      <c r="H40" s="4">
-        <f t="shared" si="13"/>
         <v>275543.09249914961</v>
       </c>
       <c r="I40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -1888,36 +1932,36 @@
         <v>5</v>
       </c>
       <c r="B41" s="4">
+        <f t="shared" si="19"/>
+        <v>275543.09249914961</v>
+      </c>
+      <c r="C41" s="4">
+        <v>15</v>
+      </c>
+      <c r="D41" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E41" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F41" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="14"/>
+        <v>40643.263874872449</v>
+      </c>
+      <c r="H41" s="9">
         <f t="shared" si="16"/>
-        <v>275543.09249914961</v>
-      </c>
-      <c r="C41" s="4">
-        <v>15</v>
-      </c>
-      <c r="D41" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E41" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F41" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G41" s="4">
-        <f>((B41/100)*C41)-F41</f>
-        <v>40643.263874872449</v>
-      </c>
-      <c r="H41" s="4">
-        <f t="shared" si="13"/>
         <v>316186.35637402209</v>
       </c>
       <c r="I41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -1926,36 +1970,36 @@
         <v>6</v>
       </c>
       <c r="B42" s="4">
+        <f t="shared" si="19"/>
+        <v>316186.35637402209</v>
+      </c>
+      <c r="C42" s="4">
+        <v>15</v>
+      </c>
+      <c r="D42" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E42" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F42" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" si="14"/>
+        <v>46739.753456103317</v>
+      </c>
+      <c r="H42" s="9">
         <f t="shared" si="16"/>
-        <v>316186.35637402209</v>
-      </c>
-      <c r="C42" s="4">
-        <v>15</v>
-      </c>
-      <c r="D42" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E42" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F42" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G42" s="4">
-        <f>((B42/100)*C42)-F42</f>
-        <v>46739.753456103317</v>
-      </c>
-      <c r="H42" s="4">
-        <f t="shared" si="13"/>
         <v>362926.10983012541</v>
       </c>
       <c r="I42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -1964,36 +2008,36 @@
         <v>7</v>
       </c>
       <c r="B43" s="4">
+        <f t="shared" si="19"/>
+        <v>362926.10983012541</v>
+      </c>
+      <c r="C43" s="4">
+        <v>15</v>
+      </c>
+      <c r="D43" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E43" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F43" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G43" s="4">
+        <f t="shared" si="14"/>
+        <v>53750.716474518813</v>
+      </c>
+      <c r="H43" s="9">
         <f t="shared" si="16"/>
-        <v>362926.10983012541</v>
-      </c>
-      <c r="C43" s="4">
-        <v>15</v>
-      </c>
-      <c r="D43" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E43" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F43" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G43" s="4">
-        <f>((B43/100)*C43)-F43</f>
-        <v>53750.716474518813</v>
-      </c>
-      <c r="H43" s="4">
-        <f t="shared" si="13"/>
         <v>416676.82630464423</v>
       </c>
       <c r="I43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2002,36 +2046,36 @@
         <v>8</v>
       </c>
       <c r="B44" s="4">
+        <f t="shared" si="19"/>
+        <v>416676.82630464423</v>
+      </c>
+      <c r="C44" s="4">
+        <v>15</v>
+      </c>
+      <c r="D44" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E44" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F44" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" si="14"/>
+        <v>61813.32394569664</v>
+      </c>
+      <c r="H44" s="9">
         <f t="shared" si="16"/>
-        <v>416676.82630464423</v>
-      </c>
-      <c r="C44" s="4">
-        <v>15</v>
-      </c>
-      <c r="D44" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E44" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F44" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G44" s="4">
-        <f>((B44/100)*C44)-F44</f>
-        <v>61813.32394569664</v>
-      </c>
-      <c r="H44" s="4">
-        <f t="shared" si="13"/>
         <v>478490.15025034087</v>
       </c>
       <c r="I44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2040,36 +2084,36 @@
         <v>9</v>
       </c>
       <c r="B45" s="4">
+        <f t="shared" si="19"/>
+        <v>478490.15025034087</v>
+      </c>
+      <c r="C45" s="4">
+        <v>15</v>
+      </c>
+      <c r="D45" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E45" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="14"/>
+        <v>71085.322537551139</v>
+      </c>
+      <c r="H45" s="9">
         <f t="shared" si="16"/>
-        <v>478490.15025034087</v>
-      </c>
-      <c r="C45" s="4">
-        <v>15</v>
-      </c>
-      <c r="D45" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E45" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F45" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G45" s="4">
-        <f>((B45/100)*C45)-F45</f>
-        <v>71085.322537551139</v>
-      </c>
-      <c r="H45" s="4">
-        <f t="shared" si="13"/>
         <v>549575.47278789198</v>
       </c>
       <c r="I45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2078,36 +2122,36 @@
         <v>10</v>
       </c>
       <c r="B46" s="4">
+        <f t="shared" si="19"/>
+        <v>549575.47278789198</v>
+      </c>
+      <c r="C46" s="4">
+        <v>15</v>
+      </c>
+      <c r="D46" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E46" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="14"/>
+        <v>81748.120918183806</v>
+      </c>
+      <c r="H46" s="9">
         <f t="shared" si="16"/>
-        <v>549575.47278789198</v>
-      </c>
-      <c r="C46" s="4">
-        <v>15</v>
-      </c>
-      <c r="D46" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E46" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F46" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G46" s="4">
-        <f>((B46/100)*C46)-F46</f>
-        <v>81748.120918183806</v>
-      </c>
-      <c r="H46" s="4">
-        <f t="shared" si="13"/>
         <v>631323.5937060758</v>
       </c>
       <c r="I46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2116,36 +2160,36 @@
         <v>11</v>
       </c>
       <c r="B47" s="4">
+        <f t="shared" si="19"/>
+        <v>631323.5937060758</v>
+      </c>
+      <c r="C47" s="4">
+        <v>15</v>
+      </c>
+      <c r="D47" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E47" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G47" s="4">
+        <f t="shared" si="14"/>
+        <v>94010.339055911376</v>
+      </c>
+      <c r="H47" s="9">
         <f t="shared" si="16"/>
-        <v>631323.5937060758</v>
-      </c>
-      <c r="C47" s="4">
-        <v>15</v>
-      </c>
-      <c r="D47" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E47" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F47" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G47" s="4">
-        <f>((B47/100)*C47)-F47</f>
-        <v>94010.339055911376</v>
-      </c>
-      <c r="H47" s="4">
-        <f t="shared" si="13"/>
         <v>725333.93276198721</v>
       </c>
       <c r="I47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2154,36 +2198,36 @@
         <v>12</v>
       </c>
       <c r="B48" s="4">
+        <f t="shared" si="19"/>
+        <v>725333.93276198721</v>
+      </c>
+      <c r="C48" s="4">
+        <v>15</v>
+      </c>
+      <c r="D48" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E48" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="15"/>
+        <v>688.2</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="14"/>
+        <v>108111.88991429808</v>
+      </c>
+      <c r="H48" s="9">
         <f t="shared" si="16"/>
-        <v>725333.93276198721</v>
-      </c>
-      <c r="C48" s="4">
-        <v>15</v>
-      </c>
-      <c r="D48" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E48" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F48" s="4">
-        <f t="shared" si="12"/>
-        <v>688.2</v>
-      </c>
-      <c r="G48" s="4">
-        <f>((B48/100)*C48)-F48</f>
-        <v>108111.88991429808</v>
-      </c>
-      <c r="H48" s="4">
-        <f t="shared" si="13"/>
         <v>833445.82267628529</v>
       </c>
       <c r="I48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.75</v>
       </c>
       <c r="J48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
     </row>
@@ -2223,7 +2267,7 @@
       <c r="G53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I53" s="6" t="s">
@@ -2255,10 +2299,10 @@
         <v>688.2</v>
       </c>
       <c r="G54" s="4">
-        <f>((B54/100)*C54)-F54</f>
+        <f t="shared" ref="G54:G65" si="20">((B54/100)*C54)-F54</f>
         <v>124328.67340144278</v>
       </c>
-      <c r="H54" s="4">
+      <c r="H54" s="9">
         <f>B54+G54</f>
         <v>957774.49607772811</v>
       </c>
@@ -2289,23 +2333,23 @@
         <v>22.19</v>
       </c>
       <c r="F55" s="4">
-        <f t="shared" ref="F55:F65" si="17">C55*(D55+E55)</f>
+        <f t="shared" ref="F55:F65" si="21">C55*(D55+E55)</f>
         <v>688.2</v>
       </c>
       <c r="G55" s="4">
-        <f>((B55/100)*C55)-F55</f>
+        <f t="shared" si="20"/>
         <v>142977.9744116592</v>
       </c>
-      <c r="H55" s="4">
-        <f t="shared" ref="H55:H65" si="18">B55+G55</f>
+      <c r="H55" s="9">
+        <f t="shared" ref="H55:H65" si="22">B55+G55</f>
         <v>1100752.4704893874</v>
       </c>
       <c r="I55">
-        <f t="shared" ref="I55:I65" si="19">C55/4</f>
+        <f t="shared" ref="I55:I65" si="23">C55/4</f>
         <v>3.75</v>
       </c>
       <c r="J55">
-        <f t="shared" ref="J55:J65" si="20">C55/15</f>
+        <f t="shared" ref="J55:J65" si="24">C55/15</f>
         <v>1</v>
       </c>
     </row>
@@ -2314,7 +2358,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="4">
-        <f t="shared" ref="B56:B65" si="21">H55</f>
+        <f t="shared" ref="B56:B65" si="25">H55</f>
         <v>1100752.4704893874</v>
       </c>
       <c r="C56" s="4">
@@ -2327,23 +2371,23 @@
         <v>22.19</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>688.2</v>
       </c>
       <c r="G56" s="4">
-        <f>((B56/100)*C56)-F56</f>
+        <f t="shared" si="20"/>
         <v>164424.6705734081</v>
       </c>
-      <c r="H56" s="4">
-        <f t="shared" si="18"/>
+      <c r="H56" s="9">
+        <f t="shared" si="22"/>
         <v>1265177.1410627954</v>
       </c>
       <c r="I56">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J56">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2352,36 +2396,36 @@
         <v>4</v>
       </c>
       <c r="B57" s="4">
+        <f t="shared" si="25"/>
+        <v>1265177.1410627954</v>
+      </c>
+      <c r="C57" s="4">
+        <v>15</v>
+      </c>
+      <c r="D57" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E57" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F57" s="4">
         <f t="shared" si="21"/>
-        <v>1265177.1410627954</v>
-      </c>
-      <c r="C57" s="4">
-        <v>15</v>
-      </c>
-      <c r="D57" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E57" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F57" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G57" s="4">
-        <f>((B57/100)*C57)-F57</f>
+        <f t="shared" si="20"/>
         <v>189088.3711594193</v>
       </c>
-      <c r="H57" s="4">
-        <f t="shared" si="18"/>
+      <c r="H57" s="9">
+        <f t="shared" si="22"/>
         <v>1454265.5122222146</v>
       </c>
       <c r="I57">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J57">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2390,36 +2434,36 @@
         <v>5</v>
       </c>
       <c r="B58" s="4">
+        <f t="shared" si="25"/>
+        <v>1454265.5122222146</v>
+      </c>
+      <c r="C58" s="4">
+        <v>15</v>
+      </c>
+      <c r="D58" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E58" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F58" s="4">
         <f t="shared" si="21"/>
-        <v>1454265.5122222146</v>
-      </c>
-      <c r="C58" s="4">
-        <v>15</v>
-      </c>
-      <c r="D58" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E58" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F58" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G58" s="4">
-        <f>((B58/100)*C58)-F58</f>
+        <f t="shared" si="20"/>
         <v>217451.62683333218</v>
       </c>
-      <c r="H58" s="4">
-        <f t="shared" si="18"/>
+      <c r="H58" s="9">
+        <f t="shared" si="22"/>
         <v>1671717.1390555468</v>
       </c>
       <c r="I58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J58">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2428,36 +2472,36 @@
         <v>6</v>
       </c>
       <c r="B59" s="4">
+        <f t="shared" si="25"/>
+        <v>1671717.1390555468</v>
+      </c>
+      <c r="C59" s="4">
+        <v>15</v>
+      </c>
+      <c r="D59" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E59" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F59" s="4">
         <f t="shared" si="21"/>
-        <v>1671717.1390555468</v>
-      </c>
-      <c r="C59" s="4">
-        <v>15</v>
-      </c>
-      <c r="D59" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E59" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F59" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G59" s="4">
-        <f>((B59/100)*C59)-F59</f>
+        <f t="shared" si="20"/>
         <v>250069.370858332</v>
       </c>
-      <c r="H59" s="4">
-        <f t="shared" si="18"/>
+      <c r="H59" s="9">
+        <f t="shared" si="22"/>
         <v>1921786.5099138787</v>
       </c>
       <c r="I59">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2466,36 +2510,36 @@
         <v>7</v>
       </c>
       <c r="B60" s="4">
+        <f t="shared" si="25"/>
+        <v>1921786.5099138787</v>
+      </c>
+      <c r="C60" s="4">
+        <v>15</v>
+      </c>
+      <c r="D60" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E60" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F60" s="4">
         <f t="shared" si="21"/>
-        <v>1921786.5099138787</v>
-      </c>
-      <c r="C60" s="4">
-        <v>15</v>
-      </c>
-      <c r="D60" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E60" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F60" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G60" s="4">
-        <f>((B60/100)*C60)-F60</f>
+        <f t="shared" si="20"/>
         <v>287579.77648708178</v>
       </c>
-      <c r="H60" s="4">
-        <f t="shared" si="18"/>
+      <c r="H60" s="9">
+        <f t="shared" si="22"/>
         <v>2209366.2864009608</v>
       </c>
       <c r="I60">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2504,36 +2548,36 @@
         <v>8</v>
       </c>
       <c r="B61" s="4">
+        <f t="shared" si="25"/>
+        <v>2209366.2864009608</v>
+      </c>
+      <c r="C61" s="4">
+        <v>15</v>
+      </c>
+      <c r="D61" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E61" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F61" s="4">
         <f t="shared" si="21"/>
-        <v>2209366.2864009608</v>
-      </c>
-      <c r="C61" s="4">
-        <v>15</v>
-      </c>
-      <c r="D61" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E61" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F61" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G61" s="4">
-        <f>((B61/100)*C61)-F61</f>
+        <f t="shared" si="20"/>
         <v>330716.74296014407</v>
       </c>
-      <c r="H61" s="4">
-        <f t="shared" si="18"/>
+      <c r="H61" s="9">
+        <f t="shared" si="22"/>
         <v>2540083.0293611046</v>
       </c>
       <c r="I61">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J61">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2542,36 +2586,36 @@
         <v>9</v>
       </c>
       <c r="B62" s="4">
+        <f t="shared" si="25"/>
+        <v>2540083.0293611046</v>
+      </c>
+      <c r="C62" s="4">
+        <v>15</v>
+      </c>
+      <c r="D62" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E62" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F62" s="4">
         <f t="shared" si="21"/>
-        <v>2540083.0293611046</v>
-      </c>
-      <c r="C62" s="4">
-        <v>15</v>
-      </c>
-      <c r="D62" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E62" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F62" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G62" s="4">
-        <f>((B62/100)*C62)-F62</f>
+        <f t="shared" si="20"/>
         <v>380324.25440416567</v>
       </c>
-      <c r="H62" s="4">
-        <f t="shared" si="18"/>
+      <c r="H62" s="9">
+        <f t="shared" si="22"/>
         <v>2920407.2837652704</v>
       </c>
       <c r="I62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2580,36 +2624,36 @@
         <v>10</v>
       </c>
       <c r="B63" s="4">
+        <f t="shared" si="25"/>
+        <v>2920407.2837652704</v>
+      </c>
+      <c r="C63" s="4">
+        <v>15</v>
+      </c>
+      <c r="D63" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E63" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F63" s="4">
         <f t="shared" si="21"/>
-        <v>2920407.2837652704</v>
-      </c>
-      <c r="C63" s="4">
-        <v>15</v>
-      </c>
-      <c r="D63" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E63" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F63" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G63" s="4">
-        <f>((B63/100)*C63)-F63</f>
+        <f t="shared" si="20"/>
         <v>437372.89256479056</v>
       </c>
-      <c r="H63" s="4">
-        <f t="shared" si="18"/>
+      <c r="H63" s="9">
+        <f t="shared" si="22"/>
         <v>3357780.1763300607</v>
       </c>
       <c r="I63">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J63">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2618,36 +2662,36 @@
         <v>11</v>
       </c>
       <c r="B64" s="4">
+        <f t="shared" si="25"/>
+        <v>3357780.1763300607</v>
+      </c>
+      <c r="C64" s="4">
+        <v>15</v>
+      </c>
+      <c r="D64" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E64" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F64" s="4">
         <f t="shared" si="21"/>
-        <v>3357780.1763300607</v>
-      </c>
-      <c r="C64" s="4">
-        <v>15</v>
-      </c>
-      <c r="D64" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E64" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F64" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G64" s="4">
-        <f>((B64/100)*C64)-F64</f>
+        <f t="shared" si="20"/>
         <v>502978.82644950913</v>
       </c>
-      <c r="H64" s="4">
-        <f t="shared" si="18"/>
+      <c r="H64" s="9">
+        <f t="shared" si="22"/>
         <v>3860759.0027795699</v>
       </c>
       <c r="I64">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J64">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2656,36 +2700,36 @@
         <v>12</v>
       </c>
       <c r="B65" s="4">
+        <f t="shared" si="25"/>
+        <v>3860759.0027795699</v>
+      </c>
+      <c r="C65" s="4">
+        <v>15</v>
+      </c>
+      <c r="D65" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E65" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F65" s="4">
         <f t="shared" si="21"/>
-        <v>3860759.0027795699</v>
-      </c>
-      <c r="C65" s="4">
-        <v>15</v>
-      </c>
-      <c r="D65" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E65" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F65" s="4">
-        <f t="shared" si="17"/>
         <v>688.2</v>
       </c>
       <c r="G65" s="4">
-        <f>((B65/100)*C65)-F65</f>
+        <f t="shared" si="20"/>
         <v>578425.65041693556</v>
       </c>
-      <c r="H65" s="4">
-        <f t="shared" si="18"/>
+      <c r="H65" s="9">
+        <f t="shared" si="22"/>
         <v>4439184.6531965053</v>
       </c>
       <c r="I65">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3.75</v>
       </c>
       <c r="J65">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
     </row>
@@ -2725,7 +2769,7 @@
       <c r="G70" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I70" s="6" t="s">
@@ -2757,10 +2801,10 @@
         <v>688.2</v>
       </c>
       <c r="G71" s="4">
-        <f>((B71/100)*C71)-F71</f>
+        <f t="shared" ref="G71:G82" si="26">((B71/100)*C71)-F71</f>
         <v>665189.49797947577</v>
       </c>
-      <c r="H71" s="4">
+      <c r="H71" s="9">
         <f>B71+G71</f>
         <v>5104374.1511759814</v>
       </c>
@@ -2791,23 +2835,23 @@
         <v>22.19</v>
       </c>
       <c r="F72" s="4">
-        <f t="shared" ref="F72:F82" si="22">C72*(D72+E72)</f>
+        <f t="shared" ref="F72:F82" si="27">C72*(D72+E72)</f>
         <v>688.2</v>
       </c>
       <c r="G72" s="4">
-        <f>((B72/100)*C72)-F72</f>
+        <f t="shared" si="26"/>
         <v>764967.92267639725</v>
       </c>
-      <c r="H72" s="4">
-        <f t="shared" ref="H72:H82" si="23">B72+G72</f>
+      <c r="H72" s="9">
+        <f t="shared" ref="H72:H82" si="28">B72+G72</f>
         <v>5869342.0738523789</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I82" si="24">C72/4</f>
+        <f t="shared" ref="I72:I82" si="29">C72/4</f>
         <v>3.75</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J82" si="25">C72/15</f>
+        <f t="shared" ref="J72:J82" si="30">C72/15</f>
         <v>1</v>
       </c>
     </row>
@@ -2816,7 +2860,7 @@
         <v>3</v>
       </c>
       <c r="B73" s="4">
-        <f t="shared" ref="B73:B82" si="26">H72</f>
+        <f t="shared" ref="B73:B82" si="31">H72</f>
         <v>5869342.0738523789</v>
       </c>
       <c r="C73" s="4">
@@ -2829,23 +2873,23 @@
         <v>22.19</v>
       </c>
       <c r="F73" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>688.2</v>
       </c>
       <c r="G73" s="4">
-        <f>((B73/100)*C73)-F73</f>
+        <f t="shared" si="26"/>
         <v>879713.11107785685</v>
       </c>
-      <c r="H73" s="4">
-        <f t="shared" si="23"/>
+      <c r="H73" s="9">
+        <f t="shared" si="28"/>
         <v>6749055.1849302361</v>
       </c>
       <c r="I73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -2854,36 +2898,36 @@
         <v>4</v>
       </c>
       <c r="B74" s="4">
+        <f t="shared" si="31"/>
+        <v>6749055.1849302361</v>
+      </c>
+      <c r="C74" s="4">
+        <v>15</v>
+      </c>
+      <c r="D74" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E74" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F74" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G74" s="4">
         <f t="shared" si="26"/>
-        <v>6749055.1849302361</v>
-      </c>
-      <c r="C74" s="4">
-        <v>15</v>
-      </c>
-      <c r="D74" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E74" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F74" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G74" s="4">
-        <f>((B74/100)*C74)-F74</f>
         <v>1011670.0777395354</v>
       </c>
-      <c r="H74" s="4">
-        <f t="shared" si="23"/>
+      <c r="H74" s="9">
+        <f t="shared" si="28"/>
         <v>7760725.2626697719</v>
       </c>
       <c r="I74">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J74">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -2892,36 +2936,36 @@
         <v>5</v>
       </c>
       <c r="B75" s="4">
+        <f t="shared" si="31"/>
+        <v>7760725.2626697719</v>
+      </c>
+      <c r="C75" s="4">
+        <v>15</v>
+      </c>
+      <c r="D75" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E75" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F75" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G75" s="4">
         <f t="shared" si="26"/>
-        <v>7760725.2626697719</v>
-      </c>
-      <c r="C75" s="4">
-        <v>15</v>
-      </c>
-      <c r="D75" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E75" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F75" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G75" s="4">
-        <f>((B75/100)*C75)-F75</f>
         <v>1163420.5894004658</v>
       </c>
-      <c r="H75" s="4">
-        <f t="shared" si="23"/>
+      <c r="H75" s="9">
+        <f t="shared" si="28"/>
         <v>8924145.8520702384</v>
       </c>
       <c r="I75">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J75">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -2930,36 +2974,36 @@
         <v>6</v>
       </c>
       <c r="B76" s="4">
+        <f t="shared" si="31"/>
+        <v>8924145.8520702384</v>
+      </c>
+      <c r="C76" s="4">
+        <v>15</v>
+      </c>
+      <c r="D76" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E76" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F76" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G76" s="4">
         <f t="shared" si="26"/>
-        <v>8924145.8520702384</v>
-      </c>
-      <c r="C76" s="4">
-        <v>15</v>
-      </c>
-      <c r="D76" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E76" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F76" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G76" s="4">
-        <f>((B76/100)*C76)-F76</f>
         <v>1337933.6778105358</v>
       </c>
-      <c r="H76" s="4">
-        <f t="shared" si="23"/>
+      <c r="H76" s="9">
+        <f t="shared" si="28"/>
         <v>10262079.529880773</v>
       </c>
       <c r="I76">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J76">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -2968,36 +3012,36 @@
         <v>7</v>
       </c>
       <c r="B77" s="4">
+        <f t="shared" si="31"/>
+        <v>10262079.529880773</v>
+      </c>
+      <c r="C77" s="4">
+        <v>15</v>
+      </c>
+      <c r="D77" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E77" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F77" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G77" s="4">
         <f t="shared" si="26"/>
-        <v>10262079.529880773</v>
-      </c>
-      <c r="C77" s="4">
-        <v>15</v>
-      </c>
-      <c r="D77" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E77" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F77" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G77" s="4">
-        <f>((B77/100)*C77)-F77</f>
         <v>1538623.7294821159</v>
       </c>
-      <c r="H77" s="4">
-        <f t="shared" si="23"/>
+      <c r="H77" s="9">
+        <f t="shared" si="28"/>
         <v>11800703.259362889</v>
       </c>
       <c r="I77">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -3006,36 +3050,36 @@
         <v>8</v>
       </c>
       <c r="B78" s="4">
+        <f t="shared" si="31"/>
+        <v>11800703.259362889</v>
+      </c>
+      <c r="C78" s="4">
+        <v>15</v>
+      </c>
+      <c r="D78" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E78" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F78" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G78" s="4">
         <f t="shared" si="26"/>
-        <v>11800703.259362889</v>
-      </c>
-      <c r="C78" s="4">
-        <v>15</v>
-      </c>
-      <c r="D78" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E78" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F78" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G78" s="4">
-        <f>((B78/100)*C78)-F78</f>
         <v>1769417.2889044336</v>
       </c>
-      <c r="H78" s="4">
-        <f t="shared" si="23"/>
+      <c r="H78" s="9">
+        <f t="shared" si="28"/>
         <v>13570120.548267324</v>
       </c>
       <c r="I78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J78">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -3044,36 +3088,36 @@
         <v>9</v>
       </c>
       <c r="B79" s="4">
+        <f t="shared" si="31"/>
+        <v>13570120.548267324</v>
+      </c>
+      <c r="C79" s="4">
+        <v>15</v>
+      </c>
+      <c r="D79" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E79" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F79" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G79" s="4">
         <f t="shared" si="26"/>
-        <v>13570120.548267324</v>
-      </c>
-      <c r="C79" s="4">
-        <v>15</v>
-      </c>
-      <c r="D79" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E79" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F79" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G79" s="4">
-        <f>((B79/100)*C79)-F79</f>
         <v>2034829.8822400987</v>
       </c>
-      <c r="H79" s="4">
-        <f t="shared" si="23"/>
+      <c r="H79" s="9">
+        <f t="shared" si="28"/>
         <v>15604950.430507421</v>
       </c>
       <c r="I79">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J79">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -3082,36 +3126,36 @@
         <v>10</v>
       </c>
       <c r="B80" s="4">
+        <f t="shared" si="31"/>
+        <v>15604950.430507421</v>
+      </c>
+      <c r="C80" s="4">
+        <v>15</v>
+      </c>
+      <c r="D80" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E80" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F80" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G80" s="4">
         <f t="shared" si="26"/>
-        <v>15604950.430507421</v>
-      </c>
-      <c r="C80" s="4">
-        <v>15</v>
-      </c>
-      <c r="D80" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E80" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F80" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G80" s="4">
-        <f>((B80/100)*C80)-F80</f>
         <v>2340054.3645761134</v>
       </c>
-      <c r="H80" s="4">
-        <f t="shared" si="23"/>
+      <c r="H80" s="9">
+        <f t="shared" si="28"/>
         <v>17945004.795083534</v>
       </c>
       <c r="I80">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J80">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -3120,36 +3164,36 @@
         <v>11</v>
       </c>
       <c r="B81" s="4">
+        <f t="shared" si="31"/>
+        <v>17945004.795083534</v>
+      </c>
+      <c r="C81" s="4">
+        <v>15</v>
+      </c>
+      <c r="D81" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E81" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F81" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G81" s="4">
         <f t="shared" si="26"/>
-        <v>17945004.795083534</v>
-      </c>
-      <c r="C81" s="4">
-        <v>15</v>
-      </c>
-      <c r="D81" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E81" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F81" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G81" s="4">
-        <f>((B81/100)*C81)-F81</f>
         <v>2691062.5192625299</v>
       </c>
-      <c r="H81" s="4">
-        <f t="shared" si="23"/>
+      <c r="H81" s="9">
+        <f t="shared" si="28"/>
         <v>20636067.314346064</v>
       </c>
       <c r="I81">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J81">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -3158,42 +3202,1049 @@
         <v>12</v>
       </c>
       <c r="B82" s="4">
+        <f t="shared" si="31"/>
+        <v>20636067.314346064</v>
+      </c>
+      <c r="C82" s="4">
+        <v>15</v>
+      </c>
+      <c r="D82" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E82" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F82" s="4">
+        <f t="shared" si="27"/>
+        <v>688.2</v>
+      </c>
+      <c r="G82" s="4">
         <f t="shared" si="26"/>
-        <v>20636067.314346064</v>
-      </c>
-      <c r="C82" s="4">
-        <v>15</v>
-      </c>
-      <c r="D82" s="4">
-        <v>23.69</v>
-      </c>
-      <c r="E82" s="4">
-        <v>22.19</v>
-      </c>
-      <c r="F82" s="4">
-        <f t="shared" si="22"/>
-        <v>688.2</v>
-      </c>
-      <c r="G82" s="4">
-        <f>((B82/100)*C82)-F82</f>
         <v>3094721.8971519098</v>
       </c>
-      <c r="H82" s="4">
-        <f t="shared" si="23"/>
+      <c r="H82" s="9">
+        <f t="shared" si="28"/>
         <v>23730789.211497974</v>
       </c>
       <c r="I82">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>3.75</v>
       </c>
       <c r="J82">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <f>H82</f>
+        <v>23730789.211497974</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" s="4">
+        <v>1</v>
+      </c>
+      <c r="B88" s="4">
+        <f>B86</f>
+        <v>23730789.211497974</v>
+      </c>
+      <c r="C88" s="4">
+        <v>15</v>
+      </c>
+      <c r="D88" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E88" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F88" s="4">
+        <f>C88*(D88+E88)</f>
+        <v>688.2</v>
+      </c>
+      <c r="G88" s="4">
+        <f t="shared" ref="G88:G99" si="32">((B88/100)*C88)-F88</f>
+        <v>3558930.181724696</v>
+      </c>
+      <c r="H88" s="9">
+        <f>B88+G88</f>
+        <v>27289719.393222671</v>
+      </c>
+      <c r="I88">
+        <f>C88/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="J88">
+        <f>C88/15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" s="4">
+        <v>2</v>
+      </c>
+      <c r="B89" s="4">
+        <f>H88</f>
+        <v>27289719.393222671</v>
+      </c>
+      <c r="C89" s="4">
+        <v>15</v>
+      </c>
+      <c r="D89" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E89" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F89" s="4">
+        <f t="shared" ref="F89:F99" si="33">C89*(D89+E89)</f>
+        <v>688.2</v>
+      </c>
+      <c r="G89" s="4">
+        <f t="shared" si="32"/>
+        <v>4092769.7089833999</v>
+      </c>
+      <c r="H89" s="9">
+        <f t="shared" ref="H89:H99" si="34">B89+G89</f>
+        <v>31382489.10220607</v>
+      </c>
+      <c r="I89">
+        <f t="shared" ref="I89:I99" si="35">C89/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="J89">
+        <f t="shared" ref="J89:J99" si="36">C89/15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" s="4">
+        <v>3</v>
+      </c>
+      <c r="B90" s="4">
+        <f t="shared" ref="B90:B99" si="37">H89</f>
+        <v>31382489.10220607</v>
+      </c>
+      <c r="C90" s="4">
+        <v>15</v>
+      </c>
+      <c r="D90" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E90" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F90" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G90" s="4">
+        <f t="shared" si="32"/>
+        <v>4706685.1653309101</v>
+      </c>
+      <c r="H90" s="9">
+        <f t="shared" si="34"/>
+        <v>36089174.267536983</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" s="4">
+        <v>4</v>
+      </c>
+      <c r="B91" s="4">
+        <f t="shared" si="37"/>
+        <v>36089174.267536983</v>
+      </c>
+      <c r="C91" s="4">
+        <v>15</v>
+      </c>
+      <c r="D91" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E91" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F91" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G91" s="4">
+        <f t="shared" si="32"/>
+        <v>5412687.9401305476</v>
+      </c>
+      <c r="H91" s="9">
+        <f t="shared" si="34"/>
+        <v>41501862.20766753</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" s="4">
+        <v>5</v>
+      </c>
+      <c r="B92" s="4">
+        <f t="shared" si="37"/>
+        <v>41501862.20766753</v>
+      </c>
+      <c r="C92" s="4">
+        <v>15</v>
+      </c>
+      <c r="D92" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E92" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F92" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G92" s="4">
+        <f t="shared" si="32"/>
+        <v>6224591.1311501293</v>
+      </c>
+      <c r="H92" s="9">
+        <f t="shared" si="34"/>
+        <v>47726453.338817656</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A93" s="4">
+        <v>6</v>
+      </c>
+      <c r="B93" s="4">
+        <f t="shared" si="37"/>
+        <v>47726453.338817656</v>
+      </c>
+      <c r="C93" s="4">
+        <v>15</v>
+      </c>
+      <c r="D93" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E93" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F93" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G93" s="4">
+        <f t="shared" si="32"/>
+        <v>7158279.8008226482</v>
+      </c>
+      <c r="H93" s="9">
+        <f t="shared" si="34"/>
+        <v>54884733.139640301</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A94" s="4">
+        <v>7</v>
+      </c>
+      <c r="B94" s="4">
+        <f t="shared" si="37"/>
+        <v>54884733.139640301</v>
+      </c>
+      <c r="C94" s="4">
+        <v>15</v>
+      </c>
+      <c r="D94" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E94" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F94" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G94" s="4">
+        <f t="shared" si="32"/>
+        <v>8232021.7709460454</v>
+      </c>
+      <c r="H94" s="9">
+        <f t="shared" si="34"/>
+        <v>63116754.91058635</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" s="4">
+        <v>8</v>
+      </c>
+      <c r="B95" s="4">
+        <f t="shared" si="37"/>
+        <v>63116754.91058635</v>
+      </c>
+      <c r="C95" s="4">
+        <v>15</v>
+      </c>
+      <c r="D95" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E95" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F95" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G95" s="4">
+        <f t="shared" si="32"/>
+        <v>9466825.0365879536</v>
+      </c>
+      <c r="H95" s="9">
+        <f t="shared" si="34"/>
+        <v>72583579.947174311</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" s="4">
+        <v>9</v>
+      </c>
+      <c r="B96" s="4">
+        <f t="shared" si="37"/>
+        <v>72583579.947174311</v>
+      </c>
+      <c r="C96" s="4">
+        <v>15</v>
+      </c>
+      <c r="D96" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E96" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F96" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G96" s="4">
+        <f t="shared" si="32"/>
+        <v>10886848.792076146</v>
+      </c>
+      <c r="H96" s="9">
+        <f t="shared" si="34"/>
+        <v>83470428.739250451</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" s="4">
+        <v>10</v>
+      </c>
+      <c r="B97" s="4">
+        <f t="shared" si="37"/>
+        <v>83470428.739250451</v>
+      </c>
+      <c r="C97" s="4">
+        <v>15</v>
+      </c>
+      <c r="D97" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E97" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F97" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G97" s="4">
+        <f t="shared" si="32"/>
+        <v>12519876.110887568</v>
+      </c>
+      <c r="H97" s="9">
+        <f t="shared" si="34"/>
+        <v>95990304.850138023</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" s="4">
+        <v>11</v>
+      </c>
+      <c r="B98" s="4">
+        <f t="shared" si="37"/>
+        <v>95990304.850138023</v>
+      </c>
+      <c r="C98" s="4">
+        <v>15</v>
+      </c>
+      <c r="D98" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E98" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F98" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G98" s="4">
+        <f t="shared" si="32"/>
+        <v>14397857.527520705</v>
+      </c>
+      <c r="H98" s="9">
+        <f t="shared" si="34"/>
+        <v>110388162.37765872</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" s="4">
+        <v>12</v>
+      </c>
+      <c r="B99" s="4">
+        <f t="shared" si="37"/>
+        <v>110388162.37765872</v>
+      </c>
+      <c r="C99" s="4">
+        <v>15</v>
+      </c>
+      <c r="D99" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E99" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F99" s="4">
+        <f t="shared" si="33"/>
+        <v>688.2</v>
+      </c>
+      <c r="G99" s="4">
+        <f t="shared" si="32"/>
+        <v>16557536.156648809</v>
+      </c>
+      <c r="H99" s="9">
+        <f t="shared" si="34"/>
+        <v>126945698.53430754</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="35"/>
+        <v>3.75</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <f>H99</f>
+        <v>126945698.53430754</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J104" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" s="4">
+        <v>1</v>
+      </c>
+      <c r="B105" s="4">
+        <f>B103</f>
+        <v>126945698.53430754</v>
+      </c>
+      <c r="C105" s="4">
+        <v>15</v>
+      </c>
+      <c r="D105" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E105" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F105" s="4">
+        <f>C105*(D105+E105)</f>
+        <v>688.2</v>
+      </c>
+      <c r="G105" s="4">
+        <f t="shared" ref="G105:G116" si="38">((B105/100)*C105)-F105</f>
+        <v>19041166.58014613</v>
+      </c>
+      <c r="H105" s="9">
+        <f>B105+G105</f>
+        <v>145986865.11445367</v>
+      </c>
+      <c r="I105">
+        <f>C105/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="J105">
+        <f>C105/15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" s="4">
+        <v>2</v>
+      </c>
+      <c r="B106" s="4">
+        <f>H105</f>
+        <v>145986865.11445367</v>
+      </c>
+      <c r="C106" s="4">
+        <v>15</v>
+      </c>
+      <c r="D106" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E106" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F106" s="4">
+        <f t="shared" ref="F106:F116" si="39">C106*(D106+E106)</f>
+        <v>688.2</v>
+      </c>
+      <c r="G106" s="4">
+        <f t="shared" si="38"/>
+        <v>21897341.56716805</v>
+      </c>
+      <c r="H106" s="9">
+        <f t="shared" ref="H106:H116" si="40">B106+G106</f>
+        <v>167884206.68162173</v>
+      </c>
+      <c r="I106">
+        <f t="shared" ref="I106:I116" si="41">C106/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="J106">
+        <f t="shared" ref="J106:J116" si="42">C106/15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" s="4">
+        <v>3</v>
+      </c>
+      <c r="B107" s="4">
+        <f t="shared" ref="B107:B116" si="43">H106</f>
+        <v>167884206.68162173</v>
+      </c>
+      <c r="C107" s="4">
+        <v>15</v>
+      </c>
+      <c r="D107" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E107" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F107" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G107" s="4">
+        <f t="shared" si="38"/>
+        <v>25181942.802243259</v>
+      </c>
+      <c r="H107" s="9">
+        <f t="shared" si="40"/>
+        <v>193066149.48386499</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" s="4">
+        <v>4</v>
+      </c>
+      <c r="B108" s="4">
+        <f t="shared" si="43"/>
+        <v>193066149.48386499</v>
+      </c>
+      <c r="C108" s="4">
+        <v>15</v>
+      </c>
+      <c r="D108" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E108" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F108" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G108" s="4">
+        <f t="shared" si="38"/>
+        <v>28959234.222579747</v>
+      </c>
+      <c r="H108" s="9">
+        <f t="shared" si="40"/>
+        <v>222025383.70644474</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A109" s="4">
+        <v>5</v>
+      </c>
+      <c r="B109" s="4">
+        <f t="shared" si="43"/>
+        <v>222025383.70644474</v>
+      </c>
+      <c r="C109" s="4">
+        <v>15</v>
+      </c>
+      <c r="D109" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E109" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F109" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G109" s="4">
+        <f t="shared" si="38"/>
+        <v>33303119.35596671</v>
+      </c>
+      <c r="H109" s="9">
+        <f t="shared" si="40"/>
+        <v>255328503.06241146</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A110" s="4">
+        <v>6</v>
+      </c>
+      <c r="B110" s="4">
+        <f t="shared" si="43"/>
+        <v>255328503.06241146</v>
+      </c>
+      <c r="C110" s="4">
+        <v>15</v>
+      </c>
+      <c r="D110" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E110" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F110" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G110" s="4">
+        <f t="shared" si="38"/>
+        <v>38298587.259361714</v>
+      </c>
+      <c r="H110" s="9">
+        <f t="shared" si="40"/>
+        <v>293627090.32177317</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A111" s="4">
+        <v>7</v>
+      </c>
+      <c r="B111" s="4">
+        <f t="shared" si="43"/>
+        <v>293627090.32177317</v>
+      </c>
+      <c r="C111" s="4">
+        <v>15</v>
+      </c>
+      <c r="D111" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E111" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F111" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G111" s="4">
+        <f t="shared" si="38"/>
+        <v>44043375.348265968</v>
+      </c>
+      <c r="H111" s="9">
+        <f t="shared" si="40"/>
+        <v>337670465.67003912</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A112" s="4">
+        <v>8</v>
+      </c>
+      <c r="B112" s="4">
+        <f t="shared" si="43"/>
+        <v>337670465.67003912</v>
+      </c>
+      <c r="C112" s="4">
+        <v>15</v>
+      </c>
+      <c r="D112" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E112" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F112" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G112" s="4">
+        <f t="shared" si="38"/>
+        <v>50649881.650505871</v>
+      </c>
+      <c r="H112" s="9">
+        <f t="shared" si="40"/>
+        <v>388320347.32054496</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A113" s="4">
+        <v>9</v>
+      </c>
+      <c r="B113" s="4">
+        <f t="shared" si="43"/>
+        <v>388320347.32054496</v>
+      </c>
+      <c r="C113" s="4">
+        <v>15</v>
+      </c>
+      <c r="D113" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E113" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F113" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G113" s="4">
+        <f t="shared" si="38"/>
+        <v>58247363.898081742</v>
+      </c>
+      <c r="H113" s="9">
+        <f t="shared" si="40"/>
+        <v>446567711.21862668</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" s="4">
+        <v>10</v>
+      </c>
+      <c r="B114" s="4">
+        <f t="shared" si="43"/>
+        <v>446567711.21862668</v>
+      </c>
+      <c r="C114" s="4">
+        <v>15</v>
+      </c>
+      <c r="D114" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E114" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F114" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G114" s="4">
+        <f t="shared" si="38"/>
+        <v>66984468.482794002</v>
+      </c>
+      <c r="H114" s="9">
+        <f t="shared" si="40"/>
+        <v>513552179.70142066</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" s="4">
+        <v>11</v>
+      </c>
+      <c r="B115" s="4">
+        <f t="shared" si="43"/>
+        <v>513552179.70142066</v>
+      </c>
+      <c r="C115" s="4">
+        <v>15</v>
+      </c>
+      <c r="D115" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E115" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F115" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G115" s="4">
+        <f t="shared" si="38"/>
+        <v>77032138.755213097</v>
+      </c>
+      <c r="H115" s="9">
+        <f t="shared" si="40"/>
+        <v>590584318.45663381</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116" s="4">
+        <v>12</v>
+      </c>
+      <c r="B116" s="4">
+        <f t="shared" si="43"/>
+        <v>590584318.45663381</v>
+      </c>
+      <c r="C116" s="4">
+        <v>15</v>
+      </c>
+      <c r="D116" s="4">
+        <v>23.69</v>
+      </c>
+      <c r="E116" s="4">
+        <v>22.19</v>
+      </c>
+      <c r="F116" s="4">
+        <f t="shared" si="39"/>
+        <v>688.2</v>
+      </c>
+      <c r="G116" s="4">
+        <f t="shared" si="38"/>
+        <v>88586959.568495065</v>
+      </c>
+      <c r="H116" s="9">
+        <f t="shared" si="40"/>
+        <v>679171278.02512884</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="41"/>
+        <v>3.75</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>